<commit_message>
Final Update before going public
</commit_message>
<xml_diff>
--- a/attendance-files/AIMLB/AIMLB Attendance - A.xlsx
+++ b/attendance-files/AIMLB/AIMLB Attendance - A.xlsx
@@ -1712,11 +1712,11 @@
       </c>
       <c r="E8" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>36</v>
@@ -1760,8 +1760,8 @@
       <c r="T8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U8" s="38" t="s">
-        <v>36</v>
+      <c r="U8" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V8" s="19"/>
       <c r="W8" s="6"/>
@@ -2077,11 +2077,11 @@
       </c>
       <c r="E13" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="36" t="s">
         <v>36</v>
@@ -2125,8 +2125,8 @@
       <c r="T13" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U13" s="38" t="s">
-        <v>36</v>
+      <c r="U13" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V13" s="19"/>
       <c r="W13" s="6"/>
@@ -2223,11 +2223,11 @@
       </c>
       <c r="E15" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="36" t="s">
         <v>36</v>
@@ -2271,8 +2271,8 @@
       <c r="T15" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="U15" s="38" t="s">
-        <v>36</v>
+      <c r="U15" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V15" s="19"/>
       <c r="W15" s="6"/>
@@ -2880,11 +2880,11 @@
       </c>
       <c r="E24" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" s="36" t="s">
         <v>36</v>
@@ -2928,8 +2928,8 @@
       <c r="T24" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U24" s="38" t="s">
-        <v>36</v>
+      <c r="U24" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V24" s="19"/>
       <c r="W24" s="6"/>
@@ -3391,11 +3391,11 @@
       </c>
       <c r="E31" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G31" s="36" t="s">
         <v>36</v>
@@ -3439,8 +3439,8 @@
       <c r="T31" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="U31" s="38" t="s">
-        <v>36</v>
+      <c r="U31" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V31" s="19"/>
       <c r="W31" s="6"/>
@@ -3464,11 +3464,11 @@
       </c>
       <c r="E32" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G32" s="36" t="s">
         <v>36</v>
@@ -3512,8 +3512,8 @@
       <c r="T32" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U32" s="38" t="s">
-        <v>36</v>
+      <c r="U32" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V32" s="19"/>
       <c r="W32" s="6"/>
@@ -3610,11 +3610,11 @@
       </c>
       <c r="E34" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" s="36" t="s">
         <v>36</v>
@@ -3658,8 +3658,8 @@
       <c r="T34" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="U34" s="38" t="s">
-        <v>36</v>
+      <c r="U34" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V34" s="19"/>
       <c r="W34" s="6"/>
@@ -3975,11 +3975,11 @@
       </c>
       <c r="E39" s="35">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" s="35">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G39" s="36" t="s">
         <v>36</v>
@@ -4023,8 +4023,8 @@
       <c r="T39" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U39" s="38" t="s">
-        <v>36</v>
+      <c r="U39" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V39" s="19"/>
       <c r="W39" s="6"/>
@@ -4194,11 +4194,11 @@
       </c>
       <c r="E42" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42" s="36" t="s">
         <v>36</v>
@@ -4242,8 +4242,8 @@
       <c r="T42" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="U42" s="38" t="s">
-        <v>36</v>
+      <c r="U42" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V42" s="19"/>
       <c r="W42" s="6"/>
@@ -4413,11 +4413,11 @@
       </c>
       <c r="E45" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G45" s="36" t="s">
         <v>36</v>
@@ -4461,8 +4461,8 @@
       <c r="T45" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="U45" s="38" t="s">
-        <v>36</v>
+      <c r="U45" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V45" s="19"/>
       <c r="W45" s="6"/>
@@ -4486,11 +4486,11 @@
       </c>
       <c r="E46" s="35">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F46" s="35">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G46" s="36" t="s">
         <v>36</v>
@@ -4534,8 +4534,8 @@
       <c r="T46" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U46" s="38" t="s">
-        <v>36</v>
+      <c r="U46" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V46" s="19"/>
       <c r="W46" s="6"/>
@@ -4778,11 +4778,11 @@
       </c>
       <c r="E50" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G50" s="36" t="s">
         <v>36</v>
@@ -4826,8 +4826,8 @@
       <c r="T50" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U50" s="38" t="s">
-        <v>36</v>
+      <c r="U50" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V50" s="19"/>
       <c r="W50" s="6"/>
@@ -4851,11 +4851,11 @@
       </c>
       <c r="E51" s="35">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F51" s="35">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G51" s="36" t="s">
         <v>36</v>
@@ -4899,8 +4899,8 @@
       <c r="T51" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U51" s="38" t="s">
-        <v>36</v>
+      <c r="U51" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V51" s="19"/>
       <c r="W51" s="6"/>
@@ -5143,11 +5143,11 @@
       </c>
       <c r="E55" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F55" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G55" s="36" t="s">
         <v>36</v>
@@ -5191,8 +5191,8 @@
       <c r="T55" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U55" s="38" t="s">
-        <v>36</v>
+      <c r="U55" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V55" s="19"/>
       <c r="W55" s="6"/>
@@ -5508,11 +5508,11 @@
       </c>
       <c r="E60" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G60" s="36" t="s">
         <v>36</v>
@@ -5556,8 +5556,8 @@
       <c r="T60" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U60" s="38" t="s">
-        <v>36</v>
+      <c r="U60" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V60" s="19"/>
       <c r="W60" s="6"/>
@@ -5800,11 +5800,11 @@
       </c>
       <c r="E64" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F64" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G64" s="36" t="s">
         <v>36</v>
@@ -5848,8 +5848,8 @@
       <c r="T64" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="U64" s="38" t="s">
-        <v>36</v>
+      <c r="U64" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V64" s="19"/>
       <c r="W64" s="6"/>
@@ -5873,11 +5873,11 @@
       </c>
       <c r="E65" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F65" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G65" s="36" t="s">
         <v>35</v>
@@ -5921,8 +5921,8 @@
       <c r="T65" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U65" s="38" t="s">
-        <v>36</v>
+      <c r="U65" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V65" s="19"/>
       <c r="W65" s="6"/>
@@ -6092,11 +6092,11 @@
       </c>
       <c r="E68" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F68" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G68" s="36" t="s">
         <v>36</v>
@@ -6140,8 +6140,8 @@
       <c r="T68" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U68" s="38" t="s">
-        <v>36</v>
+      <c r="U68" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V68" s="19"/>
       <c r="W68" s="6"/>
@@ -6165,11 +6165,11 @@
       </c>
       <c r="E69" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F69" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G69" s="36" t="s">
         <v>36</v>
@@ -6213,8 +6213,8 @@
       <c r="T69" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="U69" s="38" t="s">
-        <v>36</v>
+      <c r="U69" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V69" s="19"/>
       <c r="W69" s="6"/>
@@ -6286,7 +6286,7 @@
       <c r="T70" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U70" s="38" t="s">
+      <c r="U70" s="36" t="s">
         <v>36</v>
       </c>
       <c r="V70" s="19"/>
@@ -6311,11 +6311,11 @@
       </c>
       <c r="E71" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F71" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G71" s="36" t="s">
         <v>35</v>
@@ -6359,8 +6359,8 @@
       <c r="T71" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U71" s="38" t="s">
-        <v>36</v>
+      <c r="U71" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V71" s="19"/>
       <c r="W71" s="6"/>
@@ -6384,11 +6384,11 @@
       </c>
       <c r="E72" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F72" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G72" s="36" t="s">
         <v>36</v>
@@ -6432,8 +6432,8 @@
       <c r="T72" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U72" s="38" t="s">
-        <v>36</v>
+      <c r="U72" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V72" s="19"/>
       <c r="W72" s="6"/>
@@ -6457,11 +6457,11 @@
       </c>
       <c r="E73" s="35">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F73" s="35">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G73" s="36" t="s">
         <v>35</v>
@@ -6505,8 +6505,8 @@
       <c r="T73" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U73" s="38" t="s">
-        <v>36</v>
+      <c r="U73" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V73" s="19"/>
       <c r="W73" s="6"/>
@@ -6895,11 +6895,11 @@
       </c>
       <c r="E79" s="35">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F79" s="35">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G79" s="36" t="s">
         <v>36</v>
@@ -6943,8 +6943,8 @@
       <c r="T79" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="U79" s="38" t="s">
-        <v>36</v>
+      <c r="U79" s="36" t="s">
+        <v>35</v>
       </c>
       <c r="V79" s="19"/>
       <c r="W79" s="6"/>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="U83" s="48">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="V83" s="19"/>
       <c r="W83" s="6"/>
@@ -14022,7 +14022,7 @@
       <formula>NOT(ISERROR(SEARCH(("A"),(G7))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:P92 S7 T9 S11 T12 T15 S16 Q19 S20 R23 S25 Q26 S27 T29 R30 S31:T31 S33:S34 T34 R36 S40:T40 T42 R43 S44 T45 T48 Q49 S50 Q55:R55 R57 R60:R61 S60 S63 T64 S66:S67 R68 T69 R70 Q72 S74 R75 S77:S80 R80 T80 Q83:U83">
+  <conditionalFormatting sqref="G7:P92 S7 U8 T9 S11 T12 U13 T15:U15 S16 Q19 S20 R23 U24 S25 Q26 S27 T29 R30 S31:T31 U31:U32 S33:S34 T34:U34 R36 U39 S40:T40 T42:U42 R43 S44 T45 U45:U46 T48 Q49 S50 U50:U51 Q55:R55 U55 R57 R60:R61 S60 U60 S63 T64 U64:U65 S66:S67 R68 U68:U73 T69 R70 Q72 S74 R75 S77:S80 U79 R80 T80 Q83:U83">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(G7))))</formula>
     </cfRule>

</xml_diff>